<commit_message>
Para revisión por parte de: DR. EDUARDO LUDEÑA
</commit_message>
<xml_diff>
--- a/Presupuesto.xlsx
+++ b/Presupuesto.xlsx
@@ -32,7 +32,7 @@
     <t>Subsistencia</t>
   </si>
   <si>
-    <t> &amp; </t>
+    <t>&amp;</t>
   </si>
   <si>
     <t>Mensual</t>
@@ -44,7 +44,7 @@
     <t>.00</t>
   </si>
   <si>
-    <t> \\ \hline</t>
+    <t>\\ \hline</t>
   </si>
   <si>
     <t>Visitas Dr. Eduardo Ludeña - ESPOL – Guayaquil</t>
@@ -53,7 +53,7 @@
     <t>Pasajes Ida – Retorno</t>
   </si>
   <si>
-    <t> \\ \cline{2-5}</t>
+    <t>\\ \cline{2-5}</t>
   </si>
   <si>
     <t>Alimentación</t>
@@ -127,6 +127,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -186,21 +187,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -239,7 +236,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -248,25 +245,23 @@
     <col collapsed="false" hidden="true" max="2" min="2" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5816326530612"/>
     <col collapsed="false" hidden="true" max="4" min="4" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="true" max="8" min="8" style="2" width="0"/>
-    <col collapsed="false" hidden="true" max="9" min="9" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="true" max="9" min="8" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="true" max="11" min="11" style="2" width="0"/>
-    <col collapsed="false" hidden="true" max="12" min="12" style="0" width="0"/>
+    <col collapsed="false" hidden="true" max="12" min="11" style="0" width="0"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="53.3418367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="E1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -277,7 +272,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -289,10 +284,10 @@
       <c r="D2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -301,27 +296,27 @@
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="5" t="n">
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="n">
         <f aca="false">+G2*E2</f>
         <v>4800</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="5" t="str">
+      <c r="M2" s="4" t="str">
         <f aca="false">CONCATENATE(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2)</f>
-        <v> &amp; Mensual &amp; 6 &amp; 800.00 &amp; 4800.00 \\ \hline</v>
+        <v>&amp; Mensual &amp; 6 &amp; 800.00 &amp; 4800.00 \\ \hline</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="5"/>
       <c r="N3" s="0" t="n">
         <f aca="false">+J2</f>
         <v>4800</v>
@@ -340,7 +335,7 @@
       <c r="D4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -355,19 +350,19 @@
       <c r="I4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="5" t="n">
+      <c r="J4" s="4" t="n">
         <f aca="false">+G4*E4</f>
         <v>720</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="5" t="str">
+      <c r="M4" s="4" t="str">
         <f aca="false">CONCATENATE(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4,L4)</f>
-        <v> &amp; Pasajes Ida – Retorno &amp; 6 &amp; 120.00 &amp; 720.00 \\ \cline{2-5}</v>
+        <v>&amp; Pasajes Ida – Retorno &amp; 6 &amp; 120.00 &amp; 720.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -380,7 +375,7 @@
       <c r="D5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -395,19 +390,19 @@
       <c r="I5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="5" t="n">
+      <c r="J5" s="4" t="n">
         <f aca="false">+G5*E5</f>
         <v>240</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="5" t="str">
+      <c r="M5" s="4" t="str">
         <f aca="false">CONCATENATE(B5,C5,D5,E5,F5,G5,H5,I5,J5,K5,L5)</f>
-        <v> &amp; Alimentación &amp; 6 &amp; 40.00 &amp; 240.00 \\ \cline{2-5}</v>
+        <v>&amp; Alimentación &amp; 6 &amp; 40.00 &amp; 240.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,7 +415,7 @@
       <c r="D6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -435,19 +430,19 @@
       <c r="I6" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="4" t="n">
         <f aca="false">+G6*E6</f>
         <v>480</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="5" t="str">
+      <c r="M6" s="4" t="str">
         <f aca="false">CONCATENATE(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6)</f>
-        <v> &amp; Hospedaje &amp; 6 &amp; 80.00 &amp; 480.00 \\ \cline{2-5}</v>
+        <v>&amp; Hospedaje &amp; 6 &amp; 80.00 &amp; 480.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +455,7 @@
       <c r="D7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="0" t="n">
         <v>6</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -475,19 +470,19 @@
       <c r="I7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="5" t="n">
+      <c r="J7" s="4" t="n">
         <f aca="false">+G7*E7</f>
         <v>180</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="5" t="str">
+      <c r="M7" s="4" t="str">
         <f aca="false">CONCATENATE(B7,C7,D7,E7,F7,G7,H7,I7,J7,K7,L7)</f>
-        <v> &amp; Movilización &amp; 6 &amp; 30.00 &amp; 180.00 \\ \hline</v>
+        <v>&amp; Movilización &amp; 6 &amp; 30.00 &amp; 180.00 \\ \hline</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -509,14 +504,14 @@
       <c r="D9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>800</v>
+      <c r="G9" s="0" t="n">
+        <v>1000</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>8</v>
@@ -524,19 +519,19 @@
       <c r="I9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="4" t="n">
         <f aca="false">+G9*E9</f>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="5" t="str">
+      <c r="M9" s="4" t="str">
         <f aca="false">CONCATENATE(B9,C9,D9,E9,F9,G9,H9,I9,J9,K9,L9)</f>
-        <v> &amp; Computador Portátil &amp; 1 &amp; 800.00 &amp; 800.00 \\ \cline{2-5}</v>
+        <v>&amp;Computador Portátil&amp;1&amp;1000.00&amp;1000.00\\ \cline{2-5}</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +544,7 @@
       <c r="D10" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -564,19 +559,19 @@
       <c r="I10" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="5" t="n">
+      <c r="J10" s="4" t="n">
         <f aca="false">+G10*E10</f>
         <v>1.5</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="L10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="5" t="str">
+      <c r="M10" s="4" t="str">
         <f aca="false">CONCATENATE(B10,C10,D10,E10,F10,G10,H10,I10,J10,K10,L10)</f>
-        <v> &amp; Esferográficos &amp; 3 &amp; 0.50 &amp; 1.50 \\ \cline{2-5}</v>
+        <v>&amp; Esferográficos &amp; 3 &amp; 0.50 &amp; 1.50 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,7 +584,7 @@
       <c r="D11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -604,19 +599,19 @@
       <c r="I11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="5" t="n">
+      <c r="J11" s="4" t="n">
         <f aca="false">+G11*E11</f>
         <v>2</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="L11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="5" t="str">
+      <c r="M11" s="4" t="str">
         <f aca="false">CONCATENATE(B11,C11,D11,E11,F11,G11,H11,I11,J11,K11,L11)</f>
-        <v> &amp; Lápices &amp; 5 &amp; 0.40 &amp; 2.00 \\ \cline{2-5}</v>
+        <v>&amp; Lápices &amp; 5 &amp; 0.40 &amp; 2.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,7 +624,7 @@
       <c r="D12" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="0" t="s">
@@ -644,19 +639,19 @@
       <c r="I12" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="5" t="n">
+      <c r="J12" s="4" t="n">
         <f aca="false">+G12*E12</f>
         <v>5</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="5" t="str">
+      <c r="M12" s="4" t="str">
         <f aca="false">CONCATENATE(B12,C12,D12,E12,F12,G12,H12,I12,J12,K12,L12)</f>
-        <v> &amp; Papel Bond (Resma) &amp; 1 &amp; 5.00 &amp; 5.00 \\ \cline{2-5}</v>
+        <v>&amp; Papel Bond (Resma) &amp; 1 &amp; 5.00 &amp; 5.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +664,7 @@
       <c r="D13" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="0" t="n">
         <v>200</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -681,25 +676,25 @@
       <c r="I13" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" s="4" t="n">
         <f aca="false">+G13*E13</f>
         <v>6</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="5" t="str">
+      <c r="M13" s="4" t="str">
         <f aca="false">CONCATENATE(B13,C13,D13,E13,F13,G13,H13,I13,J13,K13,L13)</f>
-        <v> &amp; Copias &amp; 200 &amp; 0.03 &amp; 6.00 \\ \hline</v>
+        <v>&amp; Copias &amp; 200 &amp; 0.03 &amp; 6.00 \\ \hline</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N14" s="0" t="n">
-        <f aca="false">+SUM(J10:J13)</f>
-        <v>14.5</v>
+        <f aca="false">+SUM(J9:J13)</f>
+        <v>1014.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,7 +710,7 @@
       <c r="D15" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="0" t="n">
         <v>250</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -727,19 +722,19 @@
       <c r="I15" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="5" t="n">
+      <c r="J15" s="4" t="n">
         <f aca="false">+G15*E15</f>
         <v>12.5</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="L15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="5" t="str">
+      <c r="M15" s="4" t="str">
         <f aca="false">CONCATENATE(B15,C15,D15,E15,F15,G15,H15,I15,J15,K15,L15)</f>
-        <v> &amp; Artículos &amp; 250 &amp; 0.05 &amp; 12.50 \\ \cline{2-5}</v>
+        <v>&amp; Artículos &amp; 250 &amp; 0.05 &amp; 12.50 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -752,7 +747,7 @@
       <c r="D16" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="0" t="n">
         <v>250</v>
       </c>
       <c r="F16" s="0" t="s">
@@ -764,23 +759,23 @@
       <c r="I16" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" s="4" t="n">
         <f aca="false">+G16*E16</f>
         <v>12.5</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="L16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="5" t="str">
+      <c r="M16" s="4" t="str">
         <f aca="false">CONCATENATE(B16,C16,D16,E16,F16,G16,H16,I16,J16,K16,L16)</f>
-        <v> &amp; Adicionales &amp; 250 &amp; 0.05 &amp; 12.50 \\ \hline</v>
+        <v>&amp; Adicionales &amp; 250 &amp; 0.05 &amp; 12.50 \\ \hline</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M17" s="5" t="str">
+      <c r="M17" s="4" t="str">
         <f aca="false">CONCATENATE(D17,E17,F17,G17,H17,I17,J17,K17,L17)</f>
         <v/>
       </c>
@@ -802,7 +797,7 @@
       <c r="D18" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -817,19 +812,19 @@
       <c r="I18" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="5" t="n">
+      <c r="J18" s="4" t="n">
         <f aca="false">+G18*E18</f>
         <v>24</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="5" t="str">
+      <c r="M18" s="4" t="str">
         <f aca="false">CONCATENATE(B18,C18,D18,E18,F18,G18,H18,I18,J18,K18,L18)</f>
-        <v> &amp; Impresiones &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
+        <v>&amp; Impresiones &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +837,7 @@
       <c r="D19" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F19" s="0" t="s">
@@ -857,19 +852,19 @@
       <c r="I19" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="5" t="n">
+      <c r="J19" s="4" t="n">
         <f aca="false">+G19*E19</f>
         <v>9</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="5" t="str">
+      <c r="M19" s="4" t="str">
         <f aca="false">CONCATENATE(B19,C19,D19,E19,F19,G19,H19,I19,J19,K19,L19)</f>
-        <v> &amp; Espiralados &amp; 3 &amp; 3.00 &amp; 9.00 \\ \hline</v>
+        <v>&amp; Espiralados &amp; 3 &amp; 3.00 &amp; 9.00 \\ \hline</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,7 +886,7 @@
       <c r="D21" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F21" s="0" t="s">
@@ -906,19 +901,19 @@
       <c r="I21" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="5" t="n">
+      <c r="J21" s="4" t="n">
         <f aca="false">+G21*E21</f>
         <v>24</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M21" s="5" t="str">
+      <c r="M21" s="4" t="str">
         <f aca="false">CONCATENATE(B21,C21,D21,E21,F21,G21,H21,I21,J21,K21,L21)</f>
-        <v> &amp; Impresiones &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
+        <v>&amp; Impresiones &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,7 +926,7 @@
       <c r="D22" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="0" t="n">
         <v>3</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -946,19 +941,19 @@
       <c r="I22" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="5" t="n">
+      <c r="J22" s="4" t="n">
         <f aca="false">+G22*E22</f>
         <v>24</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="5" t="str">
+      <c r="M22" s="4" t="str">
         <f aca="false">CONCATENATE(B22,C22,D22,E22,F22,G22,H22,I22,J22,K22,L22)</f>
-        <v> &amp; Empastados &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
+        <v>&amp; Empastados &amp; 3 &amp; 8.00 &amp; 24.00 \\ \cline{2-5}</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -971,7 +966,7 @@
       <c r="D23" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="0" t="s">
@@ -986,19 +981,19 @@
       <c r="I23" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="5" t="n">
+      <c r="J23" s="4" t="n">
         <f aca="false">+G23*E23</f>
         <v>10</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="5" t="str">
+      <c r="M23" s="4" t="str">
         <f aca="false">CONCATENATE(B23,C23,D23,E23,F23,G23,H23,I23,J23,K23,L23)</f>
-        <v> &amp; CD &amp; 1 &amp; 10.00 &amp; 10.00 \\ \hline</v>
+        <v>&amp; CD &amp; 1 &amp; 10.00 &amp; 10.00 \\ \hline</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,29 +1012,29 @@
       <c r="F25" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>31</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="5" t="n">
+      <c r="J25" s="4" t="n">
         <f aca="false">+SUM(J2:J24)</f>
-        <v>7350.5</v>
+        <v>7550.5</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M25" s="5" t="str">
+      <c r="M25" s="4" t="str">
         <f aca="false">CONCATENATE(B25,C25,D25,E25,F25,G25,H25,I25,J25,K25,L25)</f>
-        <v> &amp;  &amp;  &amp; Total &amp; 7350.50 \\ \hline</v>
+        <v>&amp;&amp;&amp;Total&amp;7550.50\\ \hline</v>
       </c>
       <c r="N25" s="0" t="n">
         <f aca="false">+SUM(N3,N8,N14,N17,N20,N24)</f>
-        <v>6550.5</v>
+        <v>7550.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>